<commit_message>
Update custom utility ID
</commit_message>
<xml_diff>
--- a/scripts/lib/additional-utility-zips.xlsx
+++ b/scripts/lib/additional-utility-zips.xlsx
@@ -11,9 +11,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3947" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3947" uniqueCount="23">
   <si>
-    <t>Last Refresh Date :10/16/2023 10:17:33 AM</t>
+    <t>Last Refresh Date :08/27/2024</t>
   </si>
   <si>
     <t>Zip Code</t>
@@ -79,790 +79,7 @@
     <t>Not Available</t>
   </si>
   <si>
-    <t>AZ002</t>
-  </si>
-  <si>
-    <t>AZ003</t>
-  </si>
-  <si>
-    <t>AZ004</t>
-  </si>
-  <si>
-    <t>AZ005</t>
-  </si>
-  <si>
     <t>No</t>
-  </si>
-  <si>
-    <t>AZ006</t>
-  </si>
-  <si>
-    <t>AZ007</t>
-  </si>
-  <si>
-    <t>AZ008</t>
-  </si>
-  <si>
-    <t>AZ009</t>
-  </si>
-  <si>
-    <t>AZ010</t>
-  </si>
-  <si>
-    <t>AZ011</t>
-  </si>
-  <si>
-    <t>AZ012</t>
-  </si>
-  <si>
-    <t>AZ013</t>
-  </si>
-  <si>
-    <t>AZ014</t>
-  </si>
-  <si>
-    <t>AZ015</t>
-  </si>
-  <si>
-    <t>AZ016</t>
-  </si>
-  <si>
-    <t>AZ017</t>
-  </si>
-  <si>
-    <t>AZ018</t>
-  </si>
-  <si>
-    <t>AZ019</t>
-  </si>
-  <si>
-    <t>AZ020</t>
-  </si>
-  <si>
-    <t>AZ021</t>
-  </si>
-  <si>
-    <t>AZ022</t>
-  </si>
-  <si>
-    <t>AZ023</t>
-  </si>
-  <si>
-    <t>AZ024</t>
-  </si>
-  <si>
-    <t>AZ025</t>
-  </si>
-  <si>
-    <t>AZ026</t>
-  </si>
-  <si>
-    <t>AZ027</t>
-  </si>
-  <si>
-    <t>AZ028</t>
-  </si>
-  <si>
-    <t>AZ029</t>
-  </si>
-  <si>
-    <t>AZ030</t>
-  </si>
-  <si>
-    <t>AZ031</t>
-  </si>
-  <si>
-    <t>AZ032</t>
-  </si>
-  <si>
-    <t>AZ033</t>
-  </si>
-  <si>
-    <t>AZ034</t>
-  </si>
-  <si>
-    <t>AZ035</t>
-  </si>
-  <si>
-    <t>AZ036</t>
-  </si>
-  <si>
-    <t>AZ037</t>
-  </si>
-  <si>
-    <t>AZ038</t>
-  </si>
-  <si>
-    <t>AZ039</t>
-  </si>
-  <si>
-    <t>AZ040</t>
-  </si>
-  <si>
-    <t>AZ041</t>
-  </si>
-  <si>
-    <t>AZ042</t>
-  </si>
-  <si>
-    <t>AZ043</t>
-  </si>
-  <si>
-    <t>AZ044</t>
-  </si>
-  <si>
-    <t>AZ045</t>
-  </si>
-  <si>
-    <t>AZ046</t>
-  </si>
-  <si>
-    <t>AZ047</t>
-  </si>
-  <si>
-    <t>AZ048</t>
-  </si>
-  <si>
-    <t>AZ049</t>
-  </si>
-  <si>
-    <t>AZ050</t>
-  </si>
-  <si>
-    <t>AZ051</t>
-  </si>
-  <si>
-    <t>AZ052</t>
-  </si>
-  <si>
-    <t>AZ053</t>
-  </si>
-  <si>
-    <t>AZ054</t>
-  </si>
-  <si>
-    <t>AZ055</t>
-  </si>
-  <si>
-    <t>AZ056</t>
-  </si>
-  <si>
-    <t>AZ057</t>
-  </si>
-  <si>
-    <t>AZ058</t>
-  </si>
-  <si>
-    <t>AZ059</t>
-  </si>
-  <si>
-    <t>AZ060</t>
-  </si>
-  <si>
-    <t>AZ061</t>
-  </si>
-  <si>
-    <t>AZ062</t>
-  </si>
-  <si>
-    <t>AZ063</t>
-  </si>
-  <si>
-    <t>AZ064</t>
-  </si>
-  <si>
-    <t>AZ065</t>
-  </si>
-  <si>
-    <t>AZ066</t>
-  </si>
-  <si>
-    <t>AZ067</t>
-  </si>
-  <si>
-    <t>AZ068</t>
-  </si>
-  <si>
-    <t>AZ069</t>
-  </si>
-  <si>
-    <t>AZ070</t>
-  </si>
-  <si>
-    <t>AZ071</t>
-  </si>
-  <si>
-    <t>AZ072</t>
-  </si>
-  <si>
-    <t>AZ073</t>
-  </si>
-  <si>
-    <t>AZ074</t>
-  </si>
-  <si>
-    <t>AZ075</t>
-  </si>
-  <si>
-    <t>AZ076</t>
-  </si>
-  <si>
-    <t>AZ077</t>
-  </si>
-  <si>
-    <t>AZ078</t>
-  </si>
-  <si>
-    <t>AZ079</t>
-  </si>
-  <si>
-    <t>AZ080</t>
-  </si>
-  <si>
-    <t>AZ081</t>
-  </si>
-  <si>
-    <t>AZ082</t>
-  </si>
-  <si>
-    <t>AZ083</t>
-  </si>
-  <si>
-    <t>AZ084</t>
-  </si>
-  <si>
-    <t>AZ085</t>
-  </si>
-  <si>
-    <t>AZ086</t>
-  </si>
-  <si>
-    <t>AZ087</t>
-  </si>
-  <si>
-    <t>AZ088</t>
-  </si>
-  <si>
-    <t>AZ089</t>
-  </si>
-  <si>
-    <t>AZ090</t>
-  </si>
-  <si>
-    <t>AZ091</t>
-  </si>
-  <si>
-    <t>AZ092</t>
-  </si>
-  <si>
-    <t>AZ093</t>
-  </si>
-  <si>
-    <t>AZ094</t>
-  </si>
-  <si>
-    <t>AZ095</t>
-  </si>
-  <si>
-    <t>AZ096</t>
-  </si>
-  <si>
-    <t>AZ097</t>
-  </si>
-  <si>
-    <t>AZ098</t>
-  </si>
-  <si>
-    <t>AZ099</t>
-  </si>
-  <si>
-    <t>AZ100</t>
-  </si>
-  <si>
-    <t>AZ101</t>
-  </si>
-  <si>
-    <t>AZ102</t>
-  </si>
-  <si>
-    <t>AZ103</t>
-  </si>
-  <si>
-    <t>AZ104</t>
-  </si>
-  <si>
-    <t>AZ105</t>
-  </si>
-  <si>
-    <t>AZ106</t>
-  </si>
-  <si>
-    <t>AZ107</t>
-  </si>
-  <si>
-    <t>AZ108</t>
-  </si>
-  <si>
-    <t>AZ109</t>
-  </si>
-  <si>
-    <t>AZ110</t>
-  </si>
-  <si>
-    <t>AZ111</t>
-  </si>
-  <si>
-    <t>AZ112</t>
-  </si>
-  <si>
-    <t>AZ113</t>
-  </si>
-  <si>
-    <t>AZ114</t>
-  </si>
-  <si>
-    <t>AZ115</t>
-  </si>
-  <si>
-    <t>AZ116</t>
-  </si>
-  <si>
-    <t>AZ117</t>
-  </si>
-  <si>
-    <t>AZ118</t>
-  </si>
-  <si>
-    <t>AZ119</t>
-  </si>
-  <si>
-    <t>AZ120</t>
-  </si>
-  <si>
-    <t>AZ121</t>
-  </si>
-  <si>
-    <t>AZ122</t>
-  </si>
-  <si>
-    <t>AZ123</t>
-  </si>
-  <si>
-    <t>AZ124</t>
-  </si>
-  <si>
-    <t>AZ125</t>
-  </si>
-  <si>
-    <t>AZ126</t>
-  </si>
-  <si>
-    <t>AZ127</t>
-  </si>
-  <si>
-    <t>AZ128</t>
-  </si>
-  <si>
-    <t>AZ129</t>
-  </si>
-  <si>
-    <t>AZ130</t>
-  </si>
-  <si>
-    <t>AZ131</t>
-  </si>
-  <si>
-    <t>AZ132</t>
-  </si>
-  <si>
-    <t>AZ133</t>
-  </si>
-  <si>
-    <t>AZ134</t>
-  </si>
-  <si>
-    <t>AZ135</t>
-  </si>
-  <si>
-    <t>AZ136</t>
-  </si>
-  <si>
-    <t>AZ137</t>
-  </si>
-  <si>
-    <t>AZ138</t>
-  </si>
-  <si>
-    <t>AZ139</t>
-  </si>
-  <si>
-    <t>AZ140</t>
-  </si>
-  <si>
-    <t>AZ141</t>
-  </si>
-  <si>
-    <t>AZ142</t>
-  </si>
-  <si>
-    <t>AZ143</t>
-  </si>
-  <si>
-    <t>AZ144</t>
-  </si>
-  <si>
-    <t>AZ145</t>
-  </si>
-  <si>
-    <t>AZ146</t>
-  </si>
-  <si>
-    <t>AZ147</t>
-  </si>
-  <si>
-    <t>AZ148</t>
-  </si>
-  <si>
-    <t>AZ149</t>
-  </si>
-  <si>
-    <t>AZ150</t>
-  </si>
-  <si>
-    <t>AZ151</t>
-  </si>
-  <si>
-    <t>AZ152</t>
-  </si>
-  <si>
-    <t>AZ153</t>
-  </si>
-  <si>
-    <t>AZ154</t>
-  </si>
-  <si>
-    <t>AZ155</t>
-  </si>
-  <si>
-    <t>AZ156</t>
-  </si>
-  <si>
-    <t>AZ157</t>
-  </si>
-  <si>
-    <t>AZ158</t>
-  </si>
-  <si>
-    <t>AZ159</t>
-  </si>
-  <si>
-    <t>AZ160</t>
-  </si>
-  <si>
-    <t>AZ161</t>
-  </si>
-  <si>
-    <t>AZ162</t>
-  </si>
-  <si>
-    <t>AZ163</t>
-  </si>
-  <si>
-    <t>AZ164</t>
-  </si>
-  <si>
-    <t>AZ165</t>
-  </si>
-  <si>
-    <t>AZ166</t>
-  </si>
-  <si>
-    <t>AZ167</t>
-  </si>
-  <si>
-    <t>AZ168</t>
-  </si>
-  <si>
-    <t>AZ169</t>
-  </si>
-  <si>
-    <t>AZ170</t>
-  </si>
-  <si>
-    <t>AZ171</t>
-  </si>
-  <si>
-    <t>AZ172</t>
-  </si>
-  <si>
-    <t>AZ173</t>
-  </si>
-  <si>
-    <t>AZ174</t>
-  </si>
-  <si>
-    <t>AZ175</t>
-  </si>
-  <si>
-    <t>AZ176</t>
-  </si>
-  <si>
-    <t>AZ177</t>
-  </si>
-  <si>
-    <t>AZ178</t>
-  </si>
-  <si>
-    <t>AZ179</t>
-  </si>
-  <si>
-    <t>AZ180</t>
-  </si>
-  <si>
-    <t>AZ181</t>
-  </si>
-  <si>
-    <t>AZ182</t>
-  </si>
-  <si>
-    <t>AZ183</t>
-  </si>
-  <si>
-    <t>AZ184</t>
-  </si>
-  <si>
-    <t>AZ185</t>
-  </si>
-  <si>
-    <t>AZ186</t>
-  </si>
-  <si>
-    <t>AZ187</t>
-  </si>
-  <si>
-    <t>AZ188</t>
-  </si>
-  <si>
-    <t>AZ189</t>
-  </si>
-  <si>
-    <t>AZ190</t>
-  </si>
-  <si>
-    <t>AZ191</t>
-  </si>
-  <si>
-    <t>AZ192</t>
-  </si>
-  <si>
-    <t>AZ193</t>
-  </si>
-  <si>
-    <t>AZ194</t>
-  </si>
-  <si>
-    <t>AZ195</t>
-  </si>
-  <si>
-    <t>AZ196</t>
-  </si>
-  <si>
-    <t>AZ197</t>
-  </si>
-  <si>
-    <t>AZ198</t>
-  </si>
-  <si>
-    <t>AZ199</t>
-  </si>
-  <si>
-    <t>AZ200</t>
-  </si>
-  <si>
-    <t>AZ201</t>
-  </si>
-  <si>
-    <t>AZ202</t>
-  </si>
-  <si>
-    <t>AZ203</t>
-  </si>
-  <si>
-    <t>AZ204</t>
-  </si>
-  <si>
-    <t>AZ205</t>
-  </si>
-  <si>
-    <t>AZ206</t>
-  </si>
-  <si>
-    <t>AZ207</t>
-  </si>
-  <si>
-    <t>AZ208</t>
-  </si>
-  <si>
-    <t>AZ209</t>
-  </si>
-  <si>
-    <t>AZ210</t>
-  </si>
-  <si>
-    <t>AZ211</t>
-  </si>
-  <si>
-    <t>AZ212</t>
-  </si>
-  <si>
-    <t>AZ213</t>
-  </si>
-  <si>
-    <t>AZ214</t>
-  </si>
-  <si>
-    <t>AZ215</t>
-  </si>
-  <si>
-    <t>AZ216</t>
-  </si>
-  <si>
-    <t>AZ217</t>
-  </si>
-  <si>
-    <t>AZ218</t>
-  </si>
-  <si>
-    <t>AZ219</t>
-  </si>
-  <si>
-    <t>AZ220</t>
-  </si>
-  <si>
-    <t>AZ221</t>
-  </si>
-  <si>
-    <t>AZ222</t>
-  </si>
-  <si>
-    <t>AZ223</t>
-  </si>
-  <si>
-    <t>AZ224</t>
-  </si>
-  <si>
-    <t>AZ225</t>
-  </si>
-  <si>
-    <t>AZ226</t>
-  </si>
-  <si>
-    <t>AZ227</t>
-  </si>
-  <si>
-    <t>AZ228</t>
-  </si>
-  <si>
-    <t>AZ229</t>
-  </si>
-  <si>
-    <t>AZ230</t>
-  </si>
-  <si>
-    <t>AZ231</t>
-  </si>
-  <si>
-    <t>AZ232</t>
-  </si>
-  <si>
-    <t>AZ233</t>
-  </si>
-  <si>
-    <t>AZ234</t>
-  </si>
-  <si>
-    <t>AZ235</t>
-  </si>
-  <si>
-    <t>AZ236</t>
-  </si>
-  <si>
-    <t>AZ237</t>
-  </si>
-  <si>
-    <t>AZ238</t>
-  </si>
-  <si>
-    <t>AZ239</t>
-  </si>
-  <si>
-    <t>AZ240</t>
-  </si>
-  <si>
-    <t>AZ241</t>
-  </si>
-  <si>
-    <t>AZ242</t>
-  </si>
-  <si>
-    <t>AZ243</t>
-  </si>
-  <si>
-    <t>AZ244</t>
-  </si>
-  <si>
-    <t>AZ245</t>
-  </si>
-  <si>
-    <t>AZ246</t>
-  </si>
-  <si>
-    <t>AZ247</t>
-  </si>
-  <si>
-    <t>AZ248</t>
-  </si>
-  <si>
-    <t>AZ249</t>
-  </si>
-  <si>
-    <t>AZ250</t>
-  </si>
-  <si>
-    <t>AZ251</t>
-  </si>
-  <si>
-    <t>AZ252</t>
-  </si>
-  <si>
-    <t>AZ253</t>
-  </si>
-  <si>
-    <t>AZ254</t>
-  </si>
-  <si>
-    <t>AZ255</t>
-  </si>
-  <si>
-    <t>AZ256</t>
-  </si>
-  <si>
-    <t>AZ257</t>
-  </si>
-  <si>
-    <t>AZ258</t>
-  </si>
-  <si>
-    <t>AZ259</t>
-  </si>
-  <si>
-    <t>AZ260</t>
-  </si>
-  <si>
-    <t>AZ261</t>
-  </si>
-  <si>
-    <t>AZ262</t>
   </si>
 </sst>
 </file>
@@ -965,7 +182,7 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -1344,7 +561,7 @@
         <v>18</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>20</v>
@@ -1394,7 +611,7 @@
         <v>18</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>20</v>
@@ -1444,7 +661,7 @@
         <v>18</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>20</v>
@@ -1494,10 +711,10 @@
         <v>18</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>20</v>
@@ -1544,7 +761,7 @@
         <v>18</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>20</v>
@@ -1594,7 +811,7 @@
         <v>18</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>20</v>
@@ -1644,7 +861,7 @@
         <v>18</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>20</v>
@@ -1694,7 +911,7 @@
         <v>18</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>20</v>
@@ -1744,7 +961,7 @@
         <v>18</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>20</v>
@@ -1794,7 +1011,7 @@
         <v>18</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>20</v>
@@ -1844,7 +1061,7 @@
         <v>18</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>20</v>
@@ -1894,7 +1111,7 @@
         <v>18</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>20</v>
@@ -1944,7 +1161,7 @@
         <v>18</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>20</v>
@@ -1994,7 +1211,7 @@
         <v>18</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>20</v>
@@ -2044,7 +1261,7 @@
         <v>18</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>20</v>
@@ -2094,7 +1311,7 @@
         <v>18</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>20</v>
@@ -2144,7 +1361,7 @@
         <v>18</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>20</v>
@@ -2194,7 +1411,7 @@
         <v>18</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>20</v>
@@ -2244,7 +1461,7 @@
         <v>18</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>20</v>
@@ -2294,7 +1511,7 @@
         <v>18</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>20</v>
@@ -2344,7 +1561,7 @@
         <v>18</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>20</v>
@@ -2394,7 +1611,7 @@
         <v>18</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>20</v>
@@ -2444,7 +1661,7 @@
         <v>18</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>20</v>
@@ -2494,7 +1711,7 @@
         <v>18</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>20</v>
@@ -2544,7 +1761,7 @@
         <v>18</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>20</v>
@@ -2594,7 +1811,7 @@
         <v>18</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>20</v>
@@ -2644,7 +1861,7 @@
         <v>18</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>20</v>
@@ -2694,7 +1911,7 @@
         <v>18</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>20</v>
@@ -2744,10 +1961,10 @@
         <v>18</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>20</v>
@@ -2794,7 +2011,7 @@
         <v>18</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>20</v>
@@ -2844,10 +2061,10 @@
         <v>18</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F35" s="6" t="s">
         <v>20</v>
@@ -2894,10 +2111,10 @@
         <v>18</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>20</v>
@@ -2944,10 +2161,10 @@
         <v>18</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F37" s="6" t="s">
         <v>20</v>
@@ -2994,10 +2211,10 @@
         <v>18</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F38" s="6" t="s">
         <v>20</v>
@@ -3044,7 +2261,7 @@
         <v>18</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>20</v>
@@ -3094,10 +2311,10 @@
         <v>18</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>58</v>
+        <v>19</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>20</v>
@@ -3144,7 +2361,7 @@
         <v>18</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>20</v>
@@ -3194,7 +2411,7 @@
         <v>18</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>20</v>
@@ -3244,7 +2461,7 @@
         <v>18</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>20</v>
@@ -3294,10 +2511,10 @@
         <v>18</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>62</v>
+        <v>19</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F44" s="6" t="s">
         <v>20</v>
@@ -3344,7 +2561,7 @@
         <v>18</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>20</v>
@@ -3394,7 +2611,7 @@
         <v>18</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>64</v>
+        <v>19</v>
       </c>
       <c r="E46" s="6" t="s">
         <v>20</v>
@@ -3444,7 +2661,7 @@
         <v>18</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>65</v>
+        <v>19</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>20</v>
@@ -3494,7 +2711,7 @@
         <v>18</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>66</v>
+        <v>19</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>20</v>
@@ -3544,10 +2761,10 @@
         <v>18</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>67</v>
+        <v>19</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F49" s="6" t="s">
         <v>20</v>
@@ -3594,10 +2811,10 @@
         <v>18</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>68</v>
+        <v>19</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F50" s="6" t="s">
         <v>20</v>
@@ -3644,7 +2861,7 @@
         <v>18</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>69</v>
+        <v>19</v>
       </c>
       <c r="E51" s="6" t="s">
         <v>20</v>
@@ -3694,7 +2911,7 @@
         <v>18</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>70</v>
+        <v>19</v>
       </c>
       <c r="E52" s="6" t="s">
         <v>20</v>
@@ -3744,10 +2961,10 @@
         <v>18</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>71</v>
+        <v>19</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F53" s="6" t="s">
         <v>20</v>
@@ -3794,7 +3011,7 @@
         <v>18</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>72</v>
+        <v>19</v>
       </c>
       <c r="E54" s="6" t="s">
         <v>20</v>
@@ -3844,10 +3061,10 @@
         <v>18</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F55" s="6" t="s">
         <v>20</v>
@@ -3894,7 +3111,7 @@
         <v>18</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>74</v>
+        <v>19</v>
       </c>
       <c r="E56" s="6" t="s">
         <v>20</v>
@@ -3944,7 +3161,7 @@
         <v>18</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>75</v>
+        <v>19</v>
       </c>
       <c r="E57" s="6" t="s">
         <v>20</v>
@@ -3994,7 +3211,7 @@
         <v>18</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>76</v>
+        <v>19</v>
       </c>
       <c r="E58" s="6" t="s">
         <v>20</v>
@@ -4044,7 +3261,7 @@
         <v>18</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>77</v>
+        <v>19</v>
       </c>
       <c r="E59" s="6" t="s">
         <v>20</v>
@@ -4094,7 +3311,7 @@
         <v>18</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>78</v>
+        <v>19</v>
       </c>
       <c r="E60" s="6" t="s">
         <v>20</v>
@@ -4144,7 +3361,7 @@
         <v>18</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>79</v>
+        <v>19</v>
       </c>
       <c r="E61" s="6" t="s">
         <v>20</v>
@@ -4194,7 +3411,7 @@
         <v>18</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>80</v>
+        <v>19</v>
       </c>
       <c r="E62" s="6" t="s">
         <v>20</v>
@@ -4244,7 +3461,7 @@
         <v>18</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>81</v>
+        <v>19</v>
       </c>
       <c r="E63" s="6" t="s">
         <v>20</v>
@@ -4294,7 +3511,7 @@
         <v>18</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>82</v>
+        <v>19</v>
       </c>
       <c r="E64" s="6" t="s">
         <v>20</v>
@@ -4344,7 +3561,7 @@
         <v>18</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
       <c r="E65" s="6" t="s">
         <v>20</v>
@@ -4394,7 +3611,7 @@
         <v>18</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>84</v>
+        <v>19</v>
       </c>
       <c r="E66" s="6" t="s">
         <v>20</v>
@@ -4444,7 +3661,7 @@
         <v>18</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>85</v>
+        <v>19</v>
       </c>
       <c r="E67" s="6" t="s">
         <v>20</v>
@@ -4494,7 +3711,7 @@
         <v>18</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>86</v>
+        <v>19</v>
       </c>
       <c r="E68" s="6" t="s">
         <v>20</v>
@@ -4544,7 +3761,7 @@
         <v>18</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>87</v>
+        <v>19</v>
       </c>
       <c r="E69" s="6" t="s">
         <v>20</v>
@@ -4594,7 +3811,7 @@
         <v>18</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>88</v>
+        <v>19</v>
       </c>
       <c r="E70" s="6" t="s">
         <v>20</v>
@@ -4644,7 +3861,7 @@
         <v>18</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>89</v>
+        <v>19</v>
       </c>
       <c r="E71" s="6" t="s">
         <v>20</v>
@@ -4694,7 +3911,7 @@
         <v>18</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>90</v>
+        <v>19</v>
       </c>
       <c r="E72" s="6" t="s">
         <v>20</v>
@@ -4744,7 +3961,7 @@
         <v>18</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>91</v>
+        <v>19</v>
       </c>
       <c r="E73" s="6" t="s">
         <v>20</v>
@@ -4794,7 +4011,7 @@
         <v>18</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>92</v>
+        <v>19</v>
       </c>
       <c r="E74" s="6" t="s">
         <v>20</v>
@@ -4844,7 +4061,7 @@
         <v>18</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>93</v>
+        <v>19</v>
       </c>
       <c r="E75" s="6" t="s">
         <v>20</v>
@@ -4894,7 +4111,7 @@
         <v>18</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>94</v>
+        <v>19</v>
       </c>
       <c r="E76" s="6" t="s">
         <v>20</v>
@@ -4944,7 +4161,7 @@
         <v>18</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>95</v>
+        <v>19</v>
       </c>
       <c r="E77" s="6" t="s">
         <v>20</v>
@@ -4994,7 +4211,7 @@
         <v>18</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>96</v>
+        <v>19</v>
       </c>
       <c r="E78" s="6" t="s">
         <v>20</v>
@@ -5044,7 +4261,7 @@
         <v>18</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="E79" s="6" t="s">
         <v>20</v>
@@ -5094,7 +4311,7 @@
         <v>18</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>98</v>
+        <v>19</v>
       </c>
       <c r="E80" s="6" t="s">
         <v>20</v>
@@ -5144,7 +4361,7 @@
         <v>18</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>99</v>
+        <v>19</v>
       </c>
       <c r="E81" s="6" t="s">
         <v>20</v>
@@ -5194,7 +4411,7 @@
         <v>18</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>100</v>
+        <v>19</v>
       </c>
       <c r="E82" s="6" t="s">
         <v>20</v>
@@ -5244,7 +4461,7 @@
         <v>18</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
       <c r="E83" s="6" t="s">
         <v>20</v>
@@ -5294,7 +4511,7 @@
         <v>18</v>
       </c>
       <c r="D84" s="6" t="s">
-        <v>102</v>
+        <v>19</v>
       </c>
       <c r="E84" s="6" t="s">
         <v>20</v>
@@ -5344,7 +4561,7 @@
         <v>18</v>
       </c>
       <c r="D85" s="6" t="s">
-        <v>103</v>
+        <v>19</v>
       </c>
       <c r="E85" s="6" t="s">
         <v>20</v>
@@ -5394,10 +4611,10 @@
         <v>18</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>104</v>
+        <v>19</v>
       </c>
       <c r="E86" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F86" s="6" t="s">
         <v>20</v>
@@ -5444,7 +4661,7 @@
         <v>18</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>105</v>
+        <v>19</v>
       </c>
       <c r="E87" s="6" t="s">
         <v>20</v>
@@ -5494,7 +4711,7 @@
         <v>18</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>106</v>
+        <v>19</v>
       </c>
       <c r="E88" s="6" t="s">
         <v>20</v>
@@ -5544,10 +4761,10 @@
         <v>18</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>107</v>
+        <v>19</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F89" s="6" t="s">
         <v>20</v>
@@ -5594,7 +4811,7 @@
         <v>18</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>108</v>
+        <v>19</v>
       </c>
       <c r="E90" s="6" t="s">
         <v>20</v>
@@ -5644,7 +4861,7 @@
         <v>18</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>109</v>
+        <v>19</v>
       </c>
       <c r="E91" s="6" t="s">
         <v>20</v>
@@ -5694,7 +4911,7 @@
         <v>18</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>110</v>
+        <v>19</v>
       </c>
       <c r="E92" s="6" t="s">
         <v>20</v>
@@ -5744,7 +4961,7 @@
         <v>18</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>111</v>
+        <v>19</v>
       </c>
       <c r="E93" s="6" t="s">
         <v>20</v>
@@ -5794,7 +5011,7 @@
         <v>18</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>112</v>
+        <v>19</v>
       </c>
       <c r="E94" s="6" t="s">
         <v>20</v>
@@ -5844,7 +5061,7 @@
         <v>18</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="E95" s="6" t="s">
         <v>20</v>
@@ -5894,10 +5111,10 @@
         <v>18</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>114</v>
+        <v>19</v>
       </c>
       <c r="E96" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F96" s="6" t="s">
         <v>20</v>
@@ -5944,7 +5161,7 @@
         <v>18</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>115</v>
+        <v>19</v>
       </c>
       <c r="E97" s="6" t="s">
         <v>20</v>
@@ -5994,7 +5211,7 @@
         <v>18</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>116</v>
+        <v>19</v>
       </c>
       <c r="E98" s="6" t="s">
         <v>20</v>
@@ -6044,7 +5261,7 @@
         <v>18</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>117</v>
+        <v>19</v>
       </c>
       <c r="E99" s="6" t="s">
         <v>20</v>
@@ -6094,7 +5311,7 @@
         <v>18</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>118</v>
+        <v>19</v>
       </c>
       <c r="E100" s="6" t="s">
         <v>20</v>
@@ -6144,7 +5361,7 @@
         <v>18</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>119</v>
+        <v>19</v>
       </c>
       <c r="E101" s="6" t="s">
         <v>20</v>
@@ -6194,7 +5411,7 @@
         <v>18</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>120</v>
+        <v>19</v>
       </c>
       <c r="E102" s="6" t="s">
         <v>20</v>
@@ -6244,7 +5461,7 @@
         <v>18</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>121</v>
+        <v>19</v>
       </c>
       <c r="E103" s="6" t="s">
         <v>20</v>
@@ -6294,7 +5511,7 @@
         <v>18</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>122</v>
+        <v>19</v>
       </c>
       <c r="E104" s="6" t="s">
         <v>20</v>
@@ -6344,7 +5561,7 @@
         <v>18</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>123</v>
+        <v>19</v>
       </c>
       <c r="E105" s="6" t="s">
         <v>20</v>
@@ -6394,7 +5611,7 @@
         <v>18</v>
       </c>
       <c r="D106" s="6" t="s">
-        <v>124</v>
+        <v>19</v>
       </c>
       <c r="E106" s="6" t="s">
         <v>20</v>
@@ -6444,7 +5661,7 @@
         <v>18</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>125</v>
+        <v>19</v>
       </c>
       <c r="E107" s="6" t="s">
         <v>20</v>
@@ -6494,7 +5711,7 @@
         <v>18</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>126</v>
+        <v>19</v>
       </c>
       <c r="E108" s="6" t="s">
         <v>20</v>
@@ -6544,7 +5761,7 @@
         <v>18</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>127</v>
+        <v>19</v>
       </c>
       <c r="E109" s="6" t="s">
         <v>20</v>
@@ -6594,7 +5811,7 @@
         <v>18</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>128</v>
+        <v>19</v>
       </c>
       <c r="E110" s="6" t="s">
         <v>20</v>
@@ -6644,7 +5861,7 @@
         <v>18</v>
       </c>
       <c r="D111" s="6" t="s">
-        <v>129</v>
+        <v>19</v>
       </c>
       <c r="E111" s="6" t="s">
         <v>20</v>
@@ -6694,7 +5911,7 @@
         <v>18</v>
       </c>
       <c r="D112" s="6" t="s">
-        <v>130</v>
+        <v>19</v>
       </c>
       <c r="E112" s="6" t="s">
         <v>20</v>
@@ -6744,7 +5961,7 @@
         <v>18</v>
       </c>
       <c r="D113" s="6" t="s">
-        <v>131</v>
+        <v>19</v>
       </c>
       <c r="E113" s="6" t="s">
         <v>20</v>
@@ -6794,7 +6011,7 @@
         <v>18</v>
       </c>
       <c r="D114" s="6" t="s">
-        <v>132</v>
+        <v>19</v>
       </c>
       <c r="E114" s="6" t="s">
         <v>20</v>
@@ -6844,7 +6061,7 @@
         <v>18</v>
       </c>
       <c r="D115" s="6" t="s">
-        <v>133</v>
+        <v>19</v>
       </c>
       <c r="E115" s="6" t="s">
         <v>20</v>
@@ -6894,7 +6111,7 @@
         <v>18</v>
       </c>
       <c r="D116" s="6" t="s">
-        <v>134</v>
+        <v>19</v>
       </c>
       <c r="E116" s="6" t="s">
         <v>20</v>
@@ -6944,7 +6161,7 @@
         <v>18</v>
       </c>
       <c r="D117" s="6" t="s">
-        <v>135</v>
+        <v>19</v>
       </c>
       <c r="E117" s="6" t="s">
         <v>20</v>
@@ -6994,7 +6211,7 @@
         <v>18</v>
       </c>
       <c r="D118" s="6" t="s">
-        <v>136</v>
+        <v>19</v>
       </c>
       <c r="E118" s="6" t="s">
         <v>20</v>
@@ -7044,7 +6261,7 @@
         <v>18</v>
       </c>
       <c r="D119" s="6" t="s">
-        <v>137</v>
+        <v>19</v>
       </c>
       <c r="E119" s="6" t="s">
         <v>20</v>
@@ -7094,7 +6311,7 @@
         <v>18</v>
       </c>
       <c r="D120" s="6" t="s">
-        <v>138</v>
+        <v>19</v>
       </c>
       <c r="E120" s="6" t="s">
         <v>20</v>
@@ -7144,7 +6361,7 @@
         <v>18</v>
       </c>
       <c r="D121" s="6" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="E121" s="6" t="s">
         <v>20</v>
@@ -7194,7 +6411,7 @@
         <v>18</v>
       </c>
       <c r="D122" s="6" t="s">
-        <v>140</v>
+        <v>19</v>
       </c>
       <c r="E122" s="6" t="s">
         <v>20</v>
@@ -7244,7 +6461,7 @@
         <v>18</v>
       </c>
       <c r="D123" s="6" t="s">
-        <v>141</v>
+        <v>19</v>
       </c>
       <c r="E123" s="6" t="s">
         <v>20</v>
@@ -7294,7 +6511,7 @@
         <v>18</v>
       </c>
       <c r="D124" s="6" t="s">
-        <v>142</v>
+        <v>19</v>
       </c>
       <c r="E124" s="6" t="s">
         <v>20</v>
@@ -7344,7 +6561,7 @@
         <v>18</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>143</v>
+        <v>19</v>
       </c>
       <c r="E125" s="6" t="s">
         <v>20</v>
@@ -7394,7 +6611,7 @@
         <v>18</v>
       </c>
       <c r="D126" s="6" t="s">
-        <v>144</v>
+        <v>19</v>
       </c>
       <c r="E126" s="6" t="s">
         <v>20</v>
@@ -7444,7 +6661,7 @@
         <v>18</v>
       </c>
       <c r="D127" s="6" t="s">
-        <v>145</v>
+        <v>19</v>
       </c>
       <c r="E127" s="6" t="s">
         <v>20</v>
@@ -7494,7 +6711,7 @@
         <v>18</v>
       </c>
       <c r="D128" s="6" t="s">
-        <v>146</v>
+        <v>19</v>
       </c>
       <c r="E128" s="6" t="s">
         <v>20</v>
@@ -7544,7 +6761,7 @@
         <v>18</v>
       </c>
       <c r="D129" s="6" t="s">
-        <v>147</v>
+        <v>19</v>
       </c>
       <c r="E129" s="6" t="s">
         <v>20</v>
@@ -7594,7 +6811,7 @@
         <v>18</v>
       </c>
       <c r="D130" s="6" t="s">
-        <v>148</v>
+        <v>19</v>
       </c>
       <c r="E130" s="6" t="s">
         <v>20</v>
@@ -7644,7 +6861,7 @@
         <v>18</v>
       </c>
       <c r="D131" s="6" t="s">
-        <v>149</v>
+        <v>19</v>
       </c>
       <c r="E131" s="6" t="s">
         <v>20</v>
@@ -7694,7 +6911,7 @@
         <v>18</v>
       </c>
       <c r="D132" s="6" t="s">
-        <v>150</v>
+        <v>19</v>
       </c>
       <c r="E132" s="6" t="s">
         <v>20</v>
@@ -7744,7 +6961,7 @@
         <v>18</v>
       </c>
       <c r="D133" s="6" t="s">
-        <v>151</v>
+        <v>19</v>
       </c>
       <c r="E133" s="6" t="s">
         <v>20</v>
@@ -7794,7 +7011,7 @@
         <v>18</v>
       </c>
       <c r="D134" s="6" t="s">
-        <v>152</v>
+        <v>19</v>
       </c>
       <c r="E134" s="6" t="s">
         <v>20</v>
@@ -7844,7 +7061,7 @@
         <v>18</v>
       </c>
       <c r="D135" s="6" t="s">
-        <v>153</v>
+        <v>19</v>
       </c>
       <c r="E135" s="6" t="s">
         <v>20</v>
@@ -7894,7 +7111,7 @@
         <v>18</v>
       </c>
       <c r="D136" s="6" t="s">
-        <v>154</v>
+        <v>19</v>
       </c>
       <c r="E136" s="6" t="s">
         <v>20</v>
@@ -7944,7 +7161,7 @@
         <v>18</v>
       </c>
       <c r="D137" s="6" t="s">
-        <v>155</v>
+        <v>19</v>
       </c>
       <c r="E137" s="6" t="s">
         <v>20</v>
@@ -7994,7 +7211,7 @@
         <v>18</v>
       </c>
       <c r="D138" s="6" t="s">
-        <v>156</v>
+        <v>19</v>
       </c>
       <c r="E138" s="6" t="s">
         <v>20</v>
@@ -8044,7 +7261,7 @@
         <v>18</v>
       </c>
       <c r="D139" s="6" t="s">
-        <v>157</v>
+        <v>19</v>
       </c>
       <c r="E139" s="6" t="s">
         <v>20</v>
@@ -8094,7 +7311,7 @@
         <v>18</v>
       </c>
       <c r="D140" s="6" t="s">
-        <v>158</v>
+        <v>19</v>
       </c>
       <c r="E140" s="6" t="s">
         <v>20</v>
@@ -8144,7 +7361,7 @@
         <v>18</v>
       </c>
       <c r="D141" s="6" t="s">
-        <v>159</v>
+        <v>19</v>
       </c>
       <c r="E141" s="6" t="s">
         <v>20</v>
@@ -8194,7 +7411,7 @@
         <v>18</v>
       </c>
       <c r="D142" s="6" t="s">
-        <v>160</v>
+        <v>19</v>
       </c>
       <c r="E142" s="6" t="s">
         <v>20</v>
@@ -8244,7 +7461,7 @@
         <v>18</v>
       </c>
       <c r="D143" s="6" t="s">
-        <v>161</v>
+        <v>19</v>
       </c>
       <c r="E143" s="6" t="s">
         <v>20</v>
@@ -8294,7 +7511,7 @@
         <v>18</v>
       </c>
       <c r="D144" s="6" t="s">
-        <v>162</v>
+        <v>19</v>
       </c>
       <c r="E144" s="6" t="s">
         <v>20</v>
@@ -8344,7 +7561,7 @@
         <v>18</v>
       </c>
       <c r="D145" s="6" t="s">
-        <v>163</v>
+        <v>19</v>
       </c>
       <c r="E145" s="6" t="s">
         <v>20</v>
@@ -8394,7 +7611,7 @@
         <v>18</v>
       </c>
       <c r="D146" s="6" t="s">
-        <v>164</v>
+        <v>19</v>
       </c>
       <c r="E146" s="6" t="s">
         <v>20</v>
@@ -8444,7 +7661,7 @@
         <v>18</v>
       </c>
       <c r="D147" s="6" t="s">
-        <v>165</v>
+        <v>19</v>
       </c>
       <c r="E147" s="6" t="s">
         <v>20</v>
@@ -8494,7 +7711,7 @@
         <v>18</v>
       </c>
       <c r="D148" s="6" t="s">
-        <v>166</v>
+        <v>19</v>
       </c>
       <c r="E148" s="6" t="s">
         <v>20</v>
@@ -8544,7 +7761,7 @@
         <v>18</v>
       </c>
       <c r="D149" s="6" t="s">
-        <v>167</v>
+        <v>19</v>
       </c>
       <c r="E149" s="6" t="s">
         <v>20</v>
@@ -8594,7 +7811,7 @@
         <v>18</v>
       </c>
       <c r="D150" s="6" t="s">
-        <v>168</v>
+        <v>19</v>
       </c>
       <c r="E150" s="6" t="s">
         <v>20</v>
@@ -8644,10 +7861,10 @@
         <v>18</v>
       </c>
       <c r="D151" s="6" t="s">
-        <v>169</v>
+        <v>19</v>
       </c>
       <c r="E151" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F151" s="6" t="s">
         <v>20</v>
@@ -8694,7 +7911,7 @@
         <v>18</v>
       </c>
       <c r="D152" s="6" t="s">
-        <v>170</v>
+        <v>19</v>
       </c>
       <c r="E152" s="6" t="s">
         <v>20</v>
@@ -8744,7 +7961,7 @@
         <v>18</v>
       </c>
       <c r="D153" s="6" t="s">
-        <v>171</v>
+        <v>19</v>
       </c>
       <c r="E153" s="6" t="s">
         <v>20</v>
@@ -8794,7 +8011,7 @@
         <v>18</v>
       </c>
       <c r="D154" s="6" t="s">
-        <v>172</v>
+        <v>19</v>
       </c>
       <c r="E154" s="6" t="s">
         <v>20</v>
@@ -8844,10 +8061,10 @@
         <v>18</v>
       </c>
       <c r="D155" s="6" t="s">
-        <v>173</v>
+        <v>19</v>
       </c>
       <c r="E155" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F155" s="6" t="s">
         <v>20</v>
@@ -8894,7 +8111,7 @@
         <v>18</v>
       </c>
       <c r="D156" s="6" t="s">
-        <v>174</v>
+        <v>19</v>
       </c>
       <c r="E156" s="6" t="s">
         <v>20</v>
@@ -8944,7 +8161,7 @@
         <v>18</v>
       </c>
       <c r="D157" s="6" t="s">
-        <v>175</v>
+        <v>19</v>
       </c>
       <c r="E157" s="6" t="s">
         <v>20</v>
@@ -8994,7 +8211,7 @@
         <v>18</v>
       </c>
       <c r="D158" s="6" t="s">
-        <v>176</v>
+        <v>19</v>
       </c>
       <c r="E158" s="6" t="s">
         <v>20</v>
@@ -9044,7 +8261,7 @@
         <v>18</v>
       </c>
       <c r="D159" s="6" t="s">
-        <v>177</v>
+        <v>19</v>
       </c>
       <c r="E159" s="6" t="s">
         <v>20</v>
@@ -9094,7 +8311,7 @@
         <v>18</v>
       </c>
       <c r="D160" s="6" t="s">
-        <v>178</v>
+        <v>19</v>
       </c>
       <c r="E160" s="6" t="s">
         <v>20</v>
@@ -9144,7 +8361,7 @@
         <v>18</v>
       </c>
       <c r="D161" s="6" t="s">
-        <v>179</v>
+        <v>19</v>
       </c>
       <c r="E161" s="6" t="s">
         <v>20</v>
@@ -9194,7 +8411,7 @@
         <v>18</v>
       </c>
       <c r="D162" s="6" t="s">
-        <v>180</v>
+        <v>19</v>
       </c>
       <c r="E162" s="6" t="s">
         <v>20</v>
@@ -9244,7 +8461,7 @@
         <v>18</v>
       </c>
       <c r="D163" s="6" t="s">
-        <v>181</v>
+        <v>19</v>
       </c>
       <c r="E163" s="6" t="s">
         <v>20</v>
@@ -9294,7 +8511,7 @@
         <v>18</v>
       </c>
       <c r="D164" s="6" t="s">
-        <v>182</v>
+        <v>19</v>
       </c>
       <c r="E164" s="6" t="s">
         <v>20</v>
@@ -9344,7 +8561,7 @@
         <v>18</v>
       </c>
       <c r="D165" s="6" t="s">
-        <v>183</v>
+        <v>19</v>
       </c>
       <c r="E165" s="6" t="s">
         <v>20</v>
@@ -9394,7 +8611,7 @@
         <v>18</v>
       </c>
       <c r="D166" s="6" t="s">
-        <v>184</v>
+        <v>19</v>
       </c>
       <c r="E166" s="6" t="s">
         <v>20</v>
@@ -9444,7 +8661,7 @@
         <v>18</v>
       </c>
       <c r="D167" s="6" t="s">
-        <v>185</v>
+        <v>19</v>
       </c>
       <c r="E167" s="6" t="s">
         <v>20</v>
@@ -9494,7 +8711,7 @@
         <v>18</v>
       </c>
       <c r="D168" s="6" t="s">
-        <v>186</v>
+        <v>19</v>
       </c>
       <c r="E168" s="6" t="s">
         <v>20</v>
@@ -9544,7 +8761,7 @@
         <v>18</v>
       </c>
       <c r="D169" s="6" t="s">
-        <v>187</v>
+        <v>19</v>
       </c>
       <c r="E169" s="6" t="s">
         <v>20</v>
@@ -9594,7 +8811,7 @@
         <v>18</v>
       </c>
       <c r="D170" s="6" t="s">
-        <v>188</v>
+        <v>19</v>
       </c>
       <c r="E170" s="6" t="s">
         <v>20</v>
@@ -9644,7 +8861,7 @@
         <v>18</v>
       </c>
       <c r="D171" s="6" t="s">
-        <v>189</v>
+        <v>19</v>
       </c>
       <c r="E171" s="6" t="s">
         <v>20</v>
@@ -9694,7 +8911,7 @@
         <v>18</v>
       </c>
       <c r="D172" s="6" t="s">
-        <v>190</v>
+        <v>19</v>
       </c>
       <c r="E172" s="6" t="s">
         <v>20</v>
@@ -9744,7 +8961,7 @@
         <v>18</v>
       </c>
       <c r="D173" s="6" t="s">
-        <v>191</v>
+        <v>19</v>
       </c>
       <c r="E173" s="6" t="s">
         <v>20</v>
@@ -9794,7 +9011,7 @@
         <v>18</v>
       </c>
       <c r="D174" s="6" t="s">
-        <v>192</v>
+        <v>19</v>
       </c>
       <c r="E174" s="6" t="s">
         <v>20</v>
@@ -9844,7 +9061,7 @@
         <v>18</v>
       </c>
       <c r="D175" s="6" t="s">
-        <v>193</v>
+        <v>19</v>
       </c>
       <c r="E175" s="6" t="s">
         <v>20</v>
@@ -9894,7 +9111,7 @@
         <v>18</v>
       </c>
       <c r="D176" s="6" t="s">
-        <v>194</v>
+        <v>19</v>
       </c>
       <c r="E176" s="6" t="s">
         <v>20</v>
@@ -9944,7 +9161,7 @@
         <v>18</v>
       </c>
       <c r="D177" s="6" t="s">
-        <v>195</v>
+        <v>19</v>
       </c>
       <c r="E177" s="6" t="s">
         <v>20</v>
@@ -9994,7 +9211,7 @@
         <v>18</v>
       </c>
       <c r="D178" s="6" t="s">
-        <v>196</v>
+        <v>19</v>
       </c>
       <c r="E178" s="6" t="s">
         <v>20</v>
@@ -10044,7 +9261,7 @@
         <v>18</v>
       </c>
       <c r="D179" s="6" t="s">
-        <v>197</v>
+        <v>19</v>
       </c>
       <c r="E179" s="6" t="s">
         <v>20</v>
@@ -10094,7 +9311,7 @@
         <v>18</v>
       </c>
       <c r="D180" s="6" t="s">
-        <v>198</v>
+        <v>19</v>
       </c>
       <c r="E180" s="6" t="s">
         <v>20</v>
@@ -10144,7 +9361,7 @@
         <v>18</v>
       </c>
       <c r="D181" s="6" t="s">
-        <v>199</v>
+        <v>19</v>
       </c>
       <c r="E181" s="6" t="s">
         <v>20</v>
@@ -10194,7 +9411,7 @@
         <v>18</v>
       </c>
       <c r="D182" s="6" t="s">
-        <v>200</v>
+        <v>19</v>
       </c>
       <c r="E182" s="6" t="s">
         <v>20</v>
@@ -10244,7 +9461,7 @@
         <v>18</v>
       </c>
       <c r="D183" s="6" t="s">
-        <v>201</v>
+        <v>19</v>
       </c>
       <c r="E183" s="6" t="s">
         <v>20</v>
@@ -10294,7 +9511,7 @@
         <v>18</v>
       </c>
       <c r="D184" s="6" t="s">
-        <v>202</v>
+        <v>19</v>
       </c>
       <c r="E184" s="6" t="s">
         <v>20</v>
@@ -10344,7 +9561,7 @@
         <v>18</v>
       </c>
       <c r="D185" s="6" t="s">
-        <v>203</v>
+        <v>19</v>
       </c>
       <c r="E185" s="6" t="s">
         <v>20</v>
@@ -10394,7 +9611,7 @@
         <v>18</v>
       </c>
       <c r="D186" s="6" t="s">
-        <v>204</v>
+        <v>19</v>
       </c>
       <c r="E186" s="6" t="s">
         <v>20</v>
@@ -10444,7 +9661,7 @@
         <v>18</v>
       </c>
       <c r="D187" s="6" t="s">
-        <v>205</v>
+        <v>19</v>
       </c>
       <c r="E187" s="6" t="s">
         <v>20</v>
@@ -10494,7 +9711,7 @@
         <v>18</v>
       </c>
       <c r="D188" s="6" t="s">
-        <v>206</v>
+        <v>19</v>
       </c>
       <c r="E188" s="6" t="s">
         <v>20</v>
@@ -10544,7 +9761,7 @@
         <v>18</v>
       </c>
       <c r="D189" s="6" t="s">
-        <v>207</v>
+        <v>19</v>
       </c>
       <c r="E189" s="6" t="s">
         <v>20</v>
@@ -10594,7 +9811,7 @@
         <v>18</v>
       </c>
       <c r="D190" s="6" t="s">
-        <v>208</v>
+        <v>19</v>
       </c>
       <c r="E190" s="6" t="s">
         <v>20</v>
@@ -10644,7 +9861,7 @@
         <v>18</v>
       </c>
       <c r="D191" s="6" t="s">
-        <v>209</v>
+        <v>19</v>
       </c>
       <c r="E191" s="6" t="s">
         <v>20</v>
@@ -10694,7 +9911,7 @@
         <v>18</v>
       </c>
       <c r="D192" s="6" t="s">
-        <v>210</v>
+        <v>19</v>
       </c>
       <c r="E192" s="6" t="s">
         <v>20</v>
@@ -10744,7 +9961,7 @@
         <v>18</v>
       </c>
       <c r="D193" s="6" t="s">
-        <v>211</v>
+        <v>19</v>
       </c>
       <c r="E193" s="6" t="s">
         <v>20</v>
@@ -10794,7 +10011,7 @@
         <v>18</v>
       </c>
       <c r="D194" s="6" t="s">
-        <v>212</v>
+        <v>19</v>
       </c>
       <c r="E194" s="6" t="s">
         <v>20</v>
@@ -10844,7 +10061,7 @@
         <v>18</v>
       </c>
       <c r="D195" s="6" t="s">
-        <v>213</v>
+        <v>19</v>
       </c>
       <c r="E195" s="6" t="s">
         <v>20</v>
@@ -10894,7 +10111,7 @@
         <v>18</v>
       </c>
       <c r="D196" s="6" t="s">
-        <v>214</v>
+        <v>19</v>
       </c>
       <c r="E196" s="6" t="s">
         <v>20</v>
@@ -10944,7 +10161,7 @@
         <v>18</v>
       </c>
       <c r="D197" s="6" t="s">
-        <v>215</v>
+        <v>19</v>
       </c>
       <c r="E197" s="6" t="s">
         <v>20</v>
@@ -10994,7 +10211,7 @@
         <v>18</v>
       </c>
       <c r="D198" s="6" t="s">
-        <v>216</v>
+        <v>19</v>
       </c>
       <c r="E198" s="6" t="s">
         <v>20</v>
@@ -11044,7 +10261,7 @@
         <v>18</v>
       </c>
       <c r="D199" s="6" t="s">
-        <v>217</v>
+        <v>19</v>
       </c>
       <c r="E199" s="6" t="s">
         <v>20</v>
@@ -11094,7 +10311,7 @@
         <v>18</v>
       </c>
       <c r="D200" s="6" t="s">
-        <v>218</v>
+        <v>19</v>
       </c>
       <c r="E200" s="6" t="s">
         <v>20</v>
@@ -11144,7 +10361,7 @@
         <v>18</v>
       </c>
       <c r="D201" s="6" t="s">
-        <v>219</v>
+        <v>19</v>
       </c>
       <c r="E201" s="6" t="s">
         <v>20</v>
@@ -11194,7 +10411,7 @@
         <v>18</v>
       </c>
       <c r="D202" s="6" t="s">
-        <v>220</v>
+        <v>19</v>
       </c>
       <c r="E202" s="6" t="s">
         <v>20</v>
@@ -11244,7 +10461,7 @@
         <v>18</v>
       </c>
       <c r="D203" s="6" t="s">
-        <v>221</v>
+        <v>19</v>
       </c>
       <c r="E203" s="6" t="s">
         <v>20</v>
@@ -11294,7 +10511,7 @@
         <v>18</v>
       </c>
       <c r="D204" s="6" t="s">
-        <v>222</v>
+        <v>19</v>
       </c>
       <c r="E204" s="6" t="s">
         <v>20</v>
@@ -11344,7 +10561,7 @@
         <v>18</v>
       </c>
       <c r="D205" s="6" t="s">
-        <v>223</v>
+        <v>19</v>
       </c>
       <c r="E205" s="6" t="s">
         <v>20</v>
@@ -11394,7 +10611,7 @@
         <v>18</v>
       </c>
       <c r="D206" s="6" t="s">
-        <v>224</v>
+        <v>19</v>
       </c>
       <c r="E206" s="6" t="s">
         <v>20</v>
@@ -11444,7 +10661,7 @@
         <v>18</v>
       </c>
       <c r="D207" s="6" t="s">
-        <v>225</v>
+        <v>19</v>
       </c>
       <c r="E207" s="6" t="s">
         <v>20</v>
@@ -11494,7 +10711,7 @@
         <v>18</v>
       </c>
       <c r="D208" s="6" t="s">
-        <v>226</v>
+        <v>19</v>
       </c>
       <c r="E208" s="6" t="s">
         <v>20</v>
@@ -11544,7 +10761,7 @@
         <v>18</v>
       </c>
       <c r="D209" s="6" t="s">
-        <v>227</v>
+        <v>19</v>
       </c>
       <c r="E209" s="6" t="s">
         <v>20</v>
@@ -11594,7 +10811,7 @@
         <v>18</v>
       </c>
       <c r="D210" s="6" t="s">
-        <v>228</v>
+        <v>19</v>
       </c>
       <c r="E210" s="6" t="s">
         <v>20</v>
@@ -11644,7 +10861,7 @@
         <v>18</v>
       </c>
       <c r="D211" s="6" t="s">
-        <v>229</v>
+        <v>19</v>
       </c>
       <c r="E211" s="6" t="s">
         <v>20</v>
@@ -11694,7 +10911,7 @@
         <v>18</v>
       </c>
       <c r="D212" s="6" t="s">
-        <v>230</v>
+        <v>19</v>
       </c>
       <c r="E212" s="6" t="s">
         <v>20</v>
@@ -11744,7 +10961,7 @@
         <v>18</v>
       </c>
       <c r="D213" s="6" t="s">
-        <v>231</v>
+        <v>19</v>
       </c>
       <c r="E213" s="6" t="s">
         <v>20</v>
@@ -11794,7 +11011,7 @@
         <v>18</v>
       </c>
       <c r="D214" s="6" t="s">
-        <v>232</v>
+        <v>19</v>
       </c>
       <c r="E214" s="6" t="s">
         <v>20</v>
@@ -11844,7 +11061,7 @@
         <v>18</v>
       </c>
       <c r="D215" s="6" t="s">
-        <v>233</v>
+        <v>19</v>
       </c>
       <c r="E215" s="6" t="s">
         <v>20</v>
@@ -11894,7 +11111,7 @@
         <v>18</v>
       </c>
       <c r="D216" s="6" t="s">
-        <v>234</v>
+        <v>19</v>
       </c>
       <c r="E216" s="6" t="s">
         <v>20</v>
@@ -11944,7 +11161,7 @@
         <v>18</v>
       </c>
       <c r="D217" s="6" t="s">
-        <v>235</v>
+        <v>19</v>
       </c>
       <c r="E217" s="6" t="s">
         <v>20</v>
@@ -11994,7 +11211,7 @@
         <v>18</v>
       </c>
       <c r="D218" s="6" t="s">
-        <v>236</v>
+        <v>19</v>
       </c>
       <c r="E218" s="6" t="s">
         <v>20</v>
@@ -12044,7 +11261,7 @@
         <v>18</v>
       </c>
       <c r="D219" s="6" t="s">
-        <v>237</v>
+        <v>19</v>
       </c>
       <c r="E219" s="6" t="s">
         <v>20</v>
@@ -12094,7 +11311,7 @@
         <v>18</v>
       </c>
       <c r="D220" s="6" t="s">
-        <v>238</v>
+        <v>19</v>
       </c>
       <c r="E220" s="6" t="s">
         <v>20</v>
@@ -12144,7 +11361,7 @@
         <v>18</v>
       </c>
       <c r="D221" s="6" t="s">
-        <v>239</v>
+        <v>19</v>
       </c>
       <c r="E221" s="6" t="s">
         <v>20</v>
@@ -12194,7 +11411,7 @@
         <v>18</v>
       </c>
       <c r="D222" s="6" t="s">
-        <v>240</v>
+        <v>19</v>
       </c>
       <c r="E222" s="6" t="s">
         <v>20</v>
@@ -12244,7 +11461,7 @@
         <v>18</v>
       </c>
       <c r="D223" s="6" t="s">
-        <v>241</v>
+        <v>19</v>
       </c>
       <c r="E223" s="6" t="s">
         <v>20</v>
@@ -12294,7 +11511,7 @@
         <v>18</v>
       </c>
       <c r="D224" s="6" t="s">
-        <v>242</v>
+        <v>19</v>
       </c>
       <c r="E224" s="6" t="s">
         <v>20</v>
@@ -12344,7 +11561,7 @@
         <v>18</v>
       </c>
       <c r="D225" s="6" t="s">
-        <v>243</v>
+        <v>19</v>
       </c>
       <c r="E225" s="6" t="s">
         <v>20</v>
@@ -12394,7 +11611,7 @@
         <v>18</v>
       </c>
       <c r="D226" s="6" t="s">
-        <v>244</v>
+        <v>19</v>
       </c>
       <c r="E226" s="6" t="s">
         <v>20</v>
@@ -12444,7 +11661,7 @@
         <v>18</v>
       </c>
       <c r="D227" s="6" t="s">
-        <v>245</v>
+        <v>19</v>
       </c>
       <c r="E227" s="6" t="s">
         <v>20</v>
@@ -12494,7 +11711,7 @@
         <v>18</v>
       </c>
       <c r="D228" s="6" t="s">
-        <v>246</v>
+        <v>19</v>
       </c>
       <c r="E228" s="6" t="s">
         <v>20</v>
@@ -12544,7 +11761,7 @@
         <v>18</v>
       </c>
       <c r="D229" s="6" t="s">
-        <v>247</v>
+        <v>19</v>
       </c>
       <c r="E229" s="6" t="s">
         <v>20</v>
@@ -12594,7 +11811,7 @@
         <v>18</v>
       </c>
       <c r="D230" s="6" t="s">
-        <v>248</v>
+        <v>19</v>
       </c>
       <c r="E230" s="6" t="s">
         <v>20</v>
@@ -12644,7 +11861,7 @@
         <v>18</v>
       </c>
       <c r="D231" s="6" t="s">
-        <v>249</v>
+        <v>19</v>
       </c>
       <c r="E231" s="6" t="s">
         <v>20</v>
@@ -12694,7 +11911,7 @@
         <v>18</v>
       </c>
       <c r="D232" s="6" t="s">
-        <v>250</v>
+        <v>19</v>
       </c>
       <c r="E232" s="6" t="s">
         <v>20</v>
@@ -12744,7 +11961,7 @@
         <v>18</v>
       </c>
       <c r="D233" s="6" t="s">
-        <v>251</v>
+        <v>19</v>
       </c>
       <c r="E233" s="6" t="s">
         <v>20</v>
@@ -12794,7 +12011,7 @@
         <v>18</v>
       </c>
       <c r="D234" s="6" t="s">
-        <v>252</v>
+        <v>19</v>
       </c>
       <c r="E234" s="6" t="s">
         <v>20</v>
@@ -12844,7 +12061,7 @@
         <v>18</v>
       </c>
       <c r="D235" s="6" t="s">
-        <v>253</v>
+        <v>19</v>
       </c>
       <c r="E235" s="6" t="s">
         <v>20</v>
@@ -12894,7 +12111,7 @@
         <v>18</v>
       </c>
       <c r="D236" s="6" t="s">
-        <v>254</v>
+        <v>19</v>
       </c>
       <c r="E236" s="6" t="s">
         <v>20</v>
@@ -12944,7 +12161,7 @@
         <v>18</v>
       </c>
       <c r="D237" s="6" t="s">
-        <v>255</v>
+        <v>19</v>
       </c>
       <c r="E237" s="6" t="s">
         <v>20</v>
@@ -12994,7 +12211,7 @@
         <v>18</v>
       </c>
       <c r="D238" s="6" t="s">
-        <v>256</v>
+        <v>19</v>
       </c>
       <c r="E238" s="6" t="s">
         <v>20</v>
@@ -13044,7 +12261,7 @@
         <v>18</v>
       </c>
       <c r="D239" s="6" t="s">
-        <v>257</v>
+        <v>19</v>
       </c>
       <c r="E239" s="6" t="s">
         <v>20</v>
@@ -13094,7 +12311,7 @@
         <v>18</v>
       </c>
       <c r="D240" s="6" t="s">
-        <v>258</v>
+        <v>19</v>
       </c>
       <c r="E240" s="6" t="s">
         <v>20</v>
@@ -13144,7 +12361,7 @@
         <v>18</v>
       </c>
       <c r="D241" s="6" t="s">
-        <v>259</v>
+        <v>19</v>
       </c>
       <c r="E241" s="6" t="s">
         <v>20</v>
@@ -13194,7 +12411,7 @@
         <v>18</v>
       </c>
       <c r="D242" s="6" t="s">
-        <v>260</v>
+        <v>19</v>
       </c>
       <c r="E242" s="6" t="s">
         <v>20</v>
@@ -13244,7 +12461,7 @@
         <v>18</v>
       </c>
       <c r="D243" s="6" t="s">
-        <v>261</v>
+        <v>19</v>
       </c>
       <c r="E243" s="6" t="s">
         <v>20</v>
@@ -13294,7 +12511,7 @@
         <v>18</v>
       </c>
       <c r="D244" s="6" t="s">
-        <v>262</v>
+        <v>19</v>
       </c>
       <c r="E244" s="6" t="s">
         <v>20</v>
@@ -13344,7 +12561,7 @@
         <v>18</v>
       </c>
       <c r="D245" s="6" t="s">
-        <v>263</v>
+        <v>19</v>
       </c>
       <c r="E245" s="6" t="s">
         <v>20</v>
@@ -13394,7 +12611,7 @@
         <v>18</v>
       </c>
       <c r="D246" s="6" t="s">
-        <v>264</v>
+        <v>19</v>
       </c>
       <c r="E246" s="6" t="s">
         <v>20</v>
@@ -13444,7 +12661,7 @@
         <v>18</v>
       </c>
       <c r="D247" s="6" t="s">
-        <v>265</v>
+        <v>19</v>
       </c>
       <c r="E247" s="6" t="s">
         <v>20</v>
@@ -13494,7 +12711,7 @@
         <v>18</v>
       </c>
       <c r="D248" s="6" t="s">
-        <v>266</v>
+        <v>19</v>
       </c>
       <c r="E248" s="6" t="s">
         <v>20</v>
@@ -13544,7 +12761,7 @@
         <v>18</v>
       </c>
       <c r="D249" s="6" t="s">
-        <v>267</v>
+        <v>19</v>
       </c>
       <c r="E249" s="6" t="s">
         <v>20</v>
@@ -13594,7 +12811,7 @@
         <v>18</v>
       </c>
       <c r="D250" s="6" t="s">
-        <v>268</v>
+        <v>19</v>
       </c>
       <c r="E250" s="6" t="s">
         <v>20</v>
@@ -13644,7 +12861,7 @@
         <v>18</v>
       </c>
       <c r="D251" s="6" t="s">
-        <v>269</v>
+        <v>19</v>
       </c>
       <c r="E251" s="6" t="s">
         <v>20</v>
@@ -13694,7 +12911,7 @@
         <v>18</v>
       </c>
       <c r="D252" s="6" t="s">
-        <v>270</v>
+        <v>19</v>
       </c>
       <c r="E252" s="6" t="s">
         <v>20</v>
@@ -13744,7 +12961,7 @@
         <v>18</v>
       </c>
       <c r="D253" s="6" t="s">
-        <v>271</v>
+        <v>19</v>
       </c>
       <c r="E253" s="6" t="s">
         <v>20</v>
@@ -13794,7 +13011,7 @@
         <v>18</v>
       </c>
       <c r="D254" s="6" t="s">
-        <v>272</v>
+        <v>19</v>
       </c>
       <c r="E254" s="6" t="s">
         <v>20</v>
@@ -13844,7 +13061,7 @@
         <v>18</v>
       </c>
       <c r="D255" s="6" t="s">
-        <v>273</v>
+        <v>19</v>
       </c>
       <c r="E255" s="6" t="s">
         <v>20</v>
@@ -13894,7 +13111,7 @@
         <v>18</v>
       </c>
       <c r="D256" s="6" t="s">
-        <v>274</v>
+        <v>19</v>
       </c>
       <c r="E256" s="6" t="s">
         <v>20</v>
@@ -13944,7 +13161,7 @@
         <v>18</v>
       </c>
       <c r="D257" s="6" t="s">
-        <v>275</v>
+        <v>19</v>
       </c>
       <c r="E257" s="6" t="s">
         <v>20</v>
@@ -13994,7 +13211,7 @@
         <v>18</v>
       </c>
       <c r="D258" s="6" t="s">
-        <v>276</v>
+        <v>19</v>
       </c>
       <c r="E258" s="6" t="s">
         <v>20</v>
@@ -14044,7 +13261,7 @@
         <v>18</v>
       </c>
       <c r="D259" s="6" t="s">
-        <v>277</v>
+        <v>19</v>
       </c>
       <c r="E259" s="6" t="s">
         <v>20</v>
@@ -14094,7 +13311,7 @@
         <v>18</v>
       </c>
       <c r="D260" s="6" t="s">
-        <v>278</v>
+        <v>19</v>
       </c>
       <c r="E260" s="6" t="s">
         <v>20</v>
@@ -14144,7 +13361,7 @@
         <v>18</v>
       </c>
       <c r="D261" s="6" t="s">
-        <v>279</v>
+        <v>19</v>
       </c>
       <c r="E261" s="6" t="s">
         <v>20</v>
@@ -14194,7 +13411,7 @@
         <v>18</v>
       </c>
       <c r="D262" s="6" t="s">
-        <v>280</v>
+        <v>19</v>
       </c>
       <c r="E262" s="6" t="s">
         <v>20</v>
@@ -14244,7 +13461,7 @@
         <v>18</v>
       </c>
       <c r="D263" s="6" t="s">
-        <v>281</v>
+        <v>19</v>
       </c>
       <c r="E263" s="6" t="s">
         <v>20</v>
@@ -14294,7 +13511,7 @@
         <v>18</v>
       </c>
       <c r="D264" s="6" t="s">
-        <v>282</v>
+        <v>19</v>
       </c>
       <c r="E264" s="6" t="s">
         <v>20</v>
@@ -14344,7 +13561,7 @@
         <v>18</v>
       </c>
       <c r="D265" s="6" t="s">
-        <v>283</v>
+        <v>19</v>
       </c>
       <c r="E265" s="6" t="s">
         <v>20</v>

</xml_diff>